<commit_message>
Uploaded movies database with complete design
</commit_message>
<xml_diff>
--- a/data-dictionary.xlsx
+++ b/data-dictionary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Documents\Y3S3\systems development\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Documents\Y3S3\systems development\git\system-development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE35875E-4330-4B1A-ADE6-643C372AA459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E684AB1-0FE9-4FAD-8831-1528A1D0C9ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5E6BF579-92E7-48AA-9D2F-8DDAD55F64CA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="118">
   <si>
     <t>Production Companies</t>
   </si>
@@ -376,6 +376,18 @@
   </si>
   <si>
     <t>decimal(3,1)</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>Nationality</t>
+  </si>
+  <si>
+    <t>country_id</t>
+  </si>
+  <si>
+    <t>country_name</t>
   </si>
 </sst>
 </file>
@@ -770,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC970F0-7C41-404F-9997-695DE21C3CA9}">
-  <dimension ref="A1:U63"/>
+  <dimension ref="A1:U69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="56" workbookViewId="0">
-      <selection activeCell="W61" sqref="W61"/>
+    <sheetView tabSelected="1" topLeftCell="G33" zoomScale="79" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1066,11 +1078,11 @@
       <c r="S8" t="s">
         <v>7</v>
       </c>
-      <c r="T8">
+      <c r="T8" t="s">
+        <v>114</v>
+      </c>
+      <c r="U8">
         <v>6012</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
@@ -2368,7 +2380,7 @@
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="B63" t="s">
         <v>28</v>
@@ -2384,6 +2396,46 @@
       </c>
       <c r="U63">
         <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>24</v>
+      </c>
+      <c r="B64" t="s">
+        <v>10</v>
+      </c>
+      <c r="C64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C65" s="3"/>
+    </row>
+    <row r="66" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="B66" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>